<commit_message>
New openpyxl for reading Excel workbooks.
Version of Excel used by Thomas Dechevrens was causing error in
openpyxl.  Replaced with latest version, plus jdcal.py in openpyxl utils
folder.
</commit_message>
<xml_diff>
--- a/Gnarly_Landscape_Utilities/ResistanceHabitatDemo/ResistanceHabitat_Demo.xlsx
+++ b/Gnarly_Landscape_Utilities/ResistanceHabitatDemo/ResistanceHabitat_Demo.xlsx
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,7 +218,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -534,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -552,25 +551,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -581,7 +580,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
@@ -607,7 +606,7 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.5</v>
       </c>
       <c r="F3" s="1">
@@ -627,7 +626,7 @@
       <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.1</v>
       </c>
       <c r="F4" s="1">
@@ -647,7 +646,7 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0</v>
       </c>
       <c r="F5" s="1">
@@ -667,7 +666,7 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0</v>
       </c>
       <c r="F6" s="1">
@@ -690,7 +689,7 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>0</v>
       </c>
       <c r="F7" s="1">
@@ -710,7 +709,7 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>0</v>
       </c>
       <c r="F8" s="1">
@@ -730,7 +729,7 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>0</v>
       </c>
       <c r="F9" s="1">
@@ -750,7 +749,7 @@
       <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>0</v>
       </c>
       <c r="F10" s="1">
@@ -764,16 +763,16 @@
       <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>1</v>
       </c>
       <c r="F11" s="1">
@@ -787,13 +786,13 @@
       <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>1</v>
       </c>
       <c r="F12" s="1">
@@ -807,13 +806,13 @@
       <c r="A13" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>3</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>1</v>
       </c>
       <c r="F13" s="1">
@@ -827,13 +826,13 @@
       <c r="A14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>4</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>0.4</v>
       </c>
       <c r="F14" s="1">
@@ -847,13 +846,13 @@
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>5</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>1</v>
       </c>
       <c r="F15" s="1">
@@ -867,13 +866,13 @@
       <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>6</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>1</v>
       </c>
       <c r="F16" s="1">
@@ -887,13 +886,13 @@
       <c r="A17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>7</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>1</v>
       </c>
       <c r="F17" s="1">
@@ -907,13 +906,13 @@
       <c r="A18" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>8</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>0.4</v>
       </c>
       <c r="F18" s="1">
@@ -927,13 +926,13 @@
       <c r="A19" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>9</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -947,13 +946,13 @@
       <c r="A20" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>10</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>1</v>
       </c>
       <c r="F20" s="1">
@@ -967,13 +966,13 @@
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>11</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>0.4</v>
       </c>
       <c r="F21" s="1">
@@ -987,13 +986,13 @@
       <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>12</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>0.4</v>
       </c>
       <c r="F22" s="1">
@@ -1007,13 +1006,13 @@
       <c r="A23" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>13</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>0.3</v>
       </c>
       <c r="F23" s="1">
@@ -1027,13 +1026,13 @@
       <c r="A24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>14</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>0</v>
       </c>
       <c r="F24" s="1">
@@ -1047,13 +1046,13 @@
       <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>15</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>0.5</v>
       </c>
       <c r="F25" s="1">
@@ -1067,13 +1066,13 @@
       <c r="A26" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>16</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <v>0.4</v>
       </c>
       <c r="F26" s="1">
@@ -1087,13 +1086,13 @@
       <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>17</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="4">
         <v>0.3</v>
       </c>
       <c r="F27" s="1">
@@ -1107,13 +1106,13 @@
       <c r="A28" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>22</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <v>0</v>
       </c>
       <c r="F28" s="1">
@@ -1127,13 +1126,13 @@
       <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>23</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <v>0</v>
       </c>
       <c r="F29" s="1">
@@ -1147,13 +1146,13 @@
       <c r="A30" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>25</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="4">
         <v>0</v>
       </c>
       <c r="F30" s="1">
@@ -1167,13 +1166,13 @@
       <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>26</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="4">
         <v>0</v>
       </c>
       <c r="F31" s="1">
@@ -1187,13 +1186,13 @@
       <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>27</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="4">
         <v>0</v>
       </c>
       <c r="F32" s="1">
@@ -1207,13 +1206,13 @@
       <c r="A33" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>28</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="4">
         <v>0</v>
       </c>
       <c r="F33" s="1">
@@ -1227,13 +1226,13 @@
       <c r="A34" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>29</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="4">
         <v>0</v>
       </c>
       <c r="F34" s="1">
@@ -1247,13 +1246,13 @@
       <c r="A35" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>30</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="4">
         <v>0</v>
       </c>
       <c r="F35" s="1">
@@ -1267,13 +1266,13 @@
       <c r="A36" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>31</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="4">
         <v>0</v>
       </c>
       <c r="F36" s="1">
@@ -1287,13 +1286,13 @@
       <c r="A37" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="5">
         <v>32</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="4">
         <v>0</v>
       </c>
       <c r="F37" s="1">
@@ -1307,13 +1306,13 @@
       <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <v>33</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="4">
         <v>0</v>
       </c>
       <c r="F38" s="1">
@@ -1322,36 +1321,6 @@
       <c r="G38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>